<commit_message>
Made unit tests for LinkedStacks, updated LinkedStack.
</commit_message>
<xml_diff>
--- a/Task1.xlsx
+++ b/Task1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Stuff\Cal Poly Pomona\courses\Fall 2021\CS 2400\Projects\Project2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B3DCFA3-8479-47DE-9B5B-3D9E937565EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38171692-76E5-4A51-B646-6CEAC733D77F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1464" yWindow="1464" windowWidth="17280" windowHeight="8964" xr2:uid="{CC70E04F-B06C-49D6-B2E4-2F1E480AA651}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="28">
   <si>
     <t>Next Character from Infix Expression</t>
   </si>
@@ -93,39 +93,67 @@
     <t>+</t>
   </si>
   <si>
-    <t>/+</t>
-  </si>
-  <si>
     <t>d</t>
   </si>
   <si>
-    <t>ab*ca-d</t>
-  </si>
-  <si>
     <t>e</t>
   </si>
   <si>
-    <t>ab*ca-de</t>
-  </si>
-  <si>
-    <t>/+*</t>
-  </si>
-  <si>
-    <t>ab*ca-de*</t>
-  </si>
-  <si>
-    <t>ab*ca-de*+</t>
-  </si>
-  <si>
-    <t>ab*ca-de*+/</t>
+    <t>ab*ca-/</t>
+  </si>
+  <si>
+    <t>ab*ca-/d</t>
+  </si>
+  <si>
+    <t>+*</t>
+  </si>
+  <si>
+    <t>ab*ca-/de</t>
+  </si>
+  <si>
+    <t>ab*ca-/de*</t>
+  </si>
+  <si>
+    <t>ab*ca-/de*+</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Infix Expression</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: a*b/(c-a)+d*e</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -153,13 +181,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -478,7 +513,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -488,43 +523,39 @@
     <col min="3" max="3" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+    </row>
+    <row r="2" spans="1:4" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
+      <c r="D2" s="1"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
       </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
@@ -532,32 +563,32 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
         <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C7" t="s">
         <v>10</v>
@@ -565,21 +596,21 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B8" t="s">
         <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C9" t="s">
         <v>14</v>
@@ -587,89 +618,96 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>16</v>
       </c>
-      <c r="B10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>17</v>
       </c>
       <c r="C11" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>18</v>
-      </c>
       <c r="B12" t="s">
         <v>17</v>
       </c>
       <c r="C12" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B13" t="s">
         <v>21</v>
       </c>
       <c r="C13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" t="s">
         <v>22</v>
       </c>
-      <c r="B14" t="s">
-        <v>23</v>
-      </c>
       <c r="C14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>5</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="C15" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B16" t="s">
-        <v>25</v>
-      </c>
-      <c r="C16" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C17" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>